<commit_message>
block 2 and project plan
</commit_message>
<xml_diff>
--- a/ADS Plan.xlsx
+++ b/ADS Plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Schule\ADS\applied_data_science\ads\ads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23EC619B-D3BE-4E53-A526-72382B6BB87A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FB9C852-E502-4397-9DCE-E897065CEEA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1FDA21DC-18C3-4648-B9B0-C1101A6BB1A7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>Mindestanforderung an die Projektarbeit (max. 9 Punkte):</t>
   </si>
@@ -125,13 +125,34 @@
     <t>Offen</t>
   </si>
   <si>
-    <t>Web Scraping</t>
-  </si>
-  <si>
-    <t>Befehle suchen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DB iterieren und +- </t>
+    <t>siehe Unterricht Cirillo</t>
+  </si>
+  <si>
+    <t>Wer</t>
+  </si>
+  <si>
+    <t>siehe Unterricht Spindler</t>
+  </si>
+  <si>
+    <t>Michael</t>
+  </si>
+  <si>
+    <t>Sebastian</t>
+  </si>
+  <si>
+    <t>Web Scraping von Börsennachrichten</t>
+  </si>
+  <si>
+    <t>Michael (?), David (Cash), Sebastian (Yahoo Fianance)</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Timeline</t>
+  </si>
+  <si>
+    <t>Abgabedatum 28.05.</t>
   </si>
 </sst>
 </file>
@@ -198,7 +219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -218,6 +239,7 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,172 +554,197 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F03ADF68-F418-4588-8C42-6A618F466411}">
-  <dimension ref="A2:C31"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="125.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>29</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D11" s="7">
+        <v>45049</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="C21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="4" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
updated plan and code
</commit_message>
<xml_diff>
--- a/ADS Plan.xlsx
+++ b/ADS Plan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://zhaw-my.sharepoint.com/personal/trautmic_students_zhaw_ch/Documents/Master/FS23 - ADS/ADS Project/GIT/ads-14/ads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Schule\ADS\applied_data_science\ads\ads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{7B1D2D68-52D7-4CB1-8126-AA703B6C63CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3B1759B2-B178-4442-AE45-376DAA65B830}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89B7D80C-1754-414D-81A7-F0632155A047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{1FDA21DC-18C3-4648-B9B0-C1101A6BB1A7}"/>
+    <workbookView xWindow="32490" yWindow="765" windowWidth="21915" windowHeight="13935" xr2:uid="{1FDA21DC-18C3-4648-B9B0-C1101A6BB1A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
   <si>
     <t>Mindestanforderung an die Projektarbeit (max. 9 Punkte):</t>
   </si>
@@ -153,6 +153,9 @@
   </si>
   <si>
     <t>Abgabedatum 28.05.</t>
+  </si>
+  <si>
+    <t>Mit Mario besprechen</t>
   </si>
 </sst>
 </file>
@@ -242,7 +245,7 @@
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -258,7 +261,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -557,10 +560,10 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="125.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
@@ -645,6 +648,9 @@
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="C11" t="s">
+        <v>39</v>
+      </c>
       <c r="D11" s="7">
         <v>45049</v>
       </c>
@@ -693,6 +699,9 @@
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>17</v>
+      </c>
+      <c r="C20" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Changes after meeting with Mario
</commit_message>
<xml_diff>
--- a/ADS Plan.xlsx
+++ b/ADS Plan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Schule\ADS\applied_data_science\ads\ads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B458744F-C00F-4678-B4DB-B906B8FA8FF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{865365BC-5DF0-4BFC-8A69-51A113F15EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11385" xr2:uid="{1FDA21DC-18C3-4648-B9B0-C1101A6BB1A7}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{1FDA21DC-18C3-4648-B9B0-C1101A6BB1A7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="40">
   <si>
     <t>Mindestanforderung an die Projektarbeit (max. 9 Punkte):</t>
   </si>
@@ -77,9 +77,6 @@
     <t>Zusatzpunkte für Projektarbeit, falls Folgendes erfüllt (max. 7 Punkte):</t>
   </si>
   <si>
-    <t>(1) Kreativität der Umsetzung (kreativ ist alles, was in den Lektionen und Übungen nicht vorgegeben wurde)</t>
-  </si>
-  <si>
     <t>(2) Verwendung von Docker Containern (Docker Compose) für die Bearbeitung und Speicherung der Daten und die Modellierung</t>
   </si>
   <si>
@@ -150,9 +147,6 @@
   </si>
   <si>
     <t>Abgabedatum 28.05.</t>
-  </si>
-  <si>
-    <t>Mit Mario besprechen</t>
   </si>
   <si>
     <t>Vermutlich mit Z5 bereits abgedeckt?</t>
@@ -160,6 +154,9 @@
   <si>
     <t>Mit Mario besprechen
 Michael (?), David (Cash), Sebastian (Yahoo Fianance)</t>
+  </si>
+  <si>
+    <t>(1) Kreativität der Umsetzung (kreativ ist alles, was in den Lektionen und Übungen nicht vorgegeben wurde): Technische Analyse</t>
   </si>
 </sst>
 </file>
@@ -188,7 +185,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -219,6 +216,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -232,7 +235,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -252,11 +255,18 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -571,10 +581,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F03ADF68-F418-4588-8C42-6A618F466411}">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -582,11 +592,12 @@
     <col min="1" max="1" width="125.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -594,13 +605,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -618,10 +629,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>40</v>
+        <v>33</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -638,16 +649,25 @@
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
+      <c r="C8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="12">
+        <v>45059.999305555553</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>32</v>
+        <v>34</v>
+      </c>
+      <c r="D9" s="12">
+        <v>45059.999305555553</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -655,21 +675,22 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="C10" s="7"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>39</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D11" s="7">
-        <v>45049</v>
+        <v>37</v>
+      </c>
+      <c r="C11" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11" s="12">
+        <v>45059.999305555553</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -677,7 +698,13 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>37</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="12">
+        <v>45059.999305555553</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -695,89 +722,95 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="12">
+        <v>45059.999305555553</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="5" t="s">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="C19" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="5" t="s">
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C20" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
+      <c r="C21" t="s">
+        <v>34</v>
+      </c>
+      <c r="D21" s="12">
+        <v>45059.999305555553</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="C21" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="2" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>